<commit_message>
Backlog atualizado e acrescentado Sprint Backlog 2
</commit_message>
<xml_diff>
--- a/docs/backlog/Backlog.xlsx
+++ b/docs/backlog/Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizvi\OneDrive\Área de Trabalho\queijo-minas pi\queijo-minas\docs\backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB1757C-7ADD-4842-92F5-AF980B446F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F38B168-B132-4FD1-BBF7-94A3638D5497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E6DED7F9-F2EA-42C5-A892-207AE9F07EE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
   <si>
     <t>REQUISITO</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Calcula e simula o retorno financeiro do produtor e oferece uma interface mais chamativa e amigável para o cliente.</t>
   </si>
   <si>
-    <t>Importante</t>
-  </si>
-  <si>
     <t>Criação de repositório GitHub</t>
   </si>
   <si>
@@ -213,6 +210,102 @@
   </si>
   <si>
     <t>PONTO DO QUEIJO</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos do Projeto</t>
+  </si>
+  <si>
+    <t>Especificação da Dashboard</t>
+  </si>
+  <si>
+    <t>BackLog da Sprint (Demanda, Pontuação, Prioridade)</t>
+  </si>
+  <si>
+    <t>Modelagem Lógica do Projeto v1</t>
+  </si>
+  <si>
+    <t>Simular a integração do Sistema ( utilização do Sensor + Gráfico )</t>
+  </si>
+  <si>
+    <t>Usar API Local / Sensor</t>
+  </si>
+  <si>
+    <t>Instalar MYSQL na VMLinux e inserção de dados do Arduíno no MySQL na mesma máquina</t>
+  </si>
+  <si>
+    <t>Validar a solução técnica</t>
+  </si>
+  <si>
+    <t>SPRINT BACKLOG 2</t>
+  </si>
+  <si>
+    <t>Repositório contendo o código-fonte atualizado do projeto, incluindo versões e histórico + documentação atualizada.</t>
+  </si>
+  <si>
+    <t>Lista de riscos identificados, suas probabilidades, impactos e planos de mitigação.</t>
+  </si>
+  <si>
+    <t>Descrição detalhada das funcionalidades e elementos visuais da dashboard a ser desenvolvida</t>
+  </si>
+  <si>
+    <t>Página institucional básica construída com HTML, CSS e JavaScript, hospedada localmente.</t>
+  </si>
+  <si>
+    <t>Dashboard local que exibe dados em formato gráfico utilizando a biblioteca ChartJS.</t>
+  </si>
+  <si>
+    <t>Sistema local de cadastro e login de usuários, implementando conceitos de repetição e validação.</t>
+  </si>
+  <si>
+    <t>Representação visual da arquitetura técnica do projeto, mostrando componentes e suas interações.</t>
+  </si>
+  <si>
+    <t>Listagem das atividades e tarefas do projeto organizadas em sprints utilizando uma ferramenta de gestão (Trello).</t>
+  </si>
+  <si>
+    <t>Registro das demandas planejadas para a sprint, incluindo estimativas de esforço e prioridades.</t>
+  </si>
+  <si>
+    <t>Modelo lógico que descreve a estrutura dos dados e relacionamentos do projeto.</t>
+  </si>
+  <si>
+    <t>Script SQL para criar o banco de dados e suas tabelas em um ambiente local.</t>
+  </si>
+  <si>
+    <t>Demonstração da integração entre o sensor e o sistema, exibindo dados em gráfico.</t>
+  </si>
+  <si>
+    <t>Implementação de uma API local que interage com sensores para coletar e processar dados.</t>
+  </si>
+  <si>
+    <t>Configuração do MySQL em uma VM Linux, com importação de dados coletados por um Arduino.</t>
+  </si>
+  <si>
+    <t>Processo de verificação e validação da solução técnica proposta para garantir seu funcionamento e eficácia.</t>
+  </si>
+  <si>
+    <t>Descrição detalhada das funcionalidades e elementos visuais da dashboard a ser desenvolvida.</t>
+  </si>
+  <si>
+    <t>Projetos atualizado no GitHub / Documentação do Projeto Atualizada</t>
+  </si>
+  <si>
+    <t>Site Estático Institucional – Local em HTML/CSS/JavaScript</t>
+  </si>
+  <si>
+    <t>Site Estático Dashboard (Gráfico com ChartJS) - Local</t>
+  </si>
+  <si>
+    <t>Site Estático Cadastro e Login – Local ( com conceito de repetições)</t>
+  </si>
+  <si>
+    <t>Diagrama de Solução (Arquitetura Técnica do Projeto)</t>
+  </si>
+  <si>
+    <t>Atividades organizadas na ferramenta de Gestão (Sprints / Atividades)</t>
+  </si>
+  <si>
+    <t>Script de criação do Banco / Tabelas criadas em BD local</t>
   </si>
 </sst>
 </file>
@@ -241,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,18 +355,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFF461"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -394,11 +481,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -409,9 +505,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -426,9 +519,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -454,17 +544,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -806,35 +909,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06753D1B-5F95-44E8-8917-CD6094E66D47}">
-  <dimension ref="B1:D35"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="45.26953125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="45.26953125" style="7" customWidth="1"/>
     <col min="3" max="3" width="110.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" style="6" customWidth="1"/>
     <col min="5" max="5" width="36.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="26" x14ac:dyDescent="0.6">
-      <c r="B1" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="21" t="s">
         <v>2</v>
       </c>
     </row>
@@ -845,7 +946,7 @@
       <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -856,7 +957,7 @@
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -867,7 +968,7 @@
       <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -878,7 +979,7 @@
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -889,282 +990,677 @@
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>14</v>
+      <c r="D7" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>21</v>
+      <c r="D11" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>21</v>
+      <c r="D22" s="11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B24" s="8" t="s">
+      <c r="C24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B26" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="D26" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B27" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="D27" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="B28" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="B28" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>14</v>
+      <c r="D28" s="19" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B29" s="4"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B30" s="2"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="B30" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B35" s="2"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
+      <c r="B32" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B35" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B36" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="29"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="27"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="27"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="1:5" ht="26" x14ac:dyDescent="0.6">
+      <c r="B45" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B46" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B47" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B48" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B50" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B51" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B52" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B53" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B56" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="27"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="27"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" s="27"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="27"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="27"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B66" s="27"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="27"/>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="27"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B68" s="27"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="27"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="27"/>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B70" s="27"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="27"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="27"/>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="27"/>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="27"/>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="27"/>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="27"/>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:D28">
     <sortCondition ref="B3:B28"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>